<commit_message>
Added documentation for python models
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CS4360\project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA194CB6-64FA-4155-94DB-7208BE4253C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA9DE4F-C914-46E1-A806-5B65CBBAF5DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22944" yWindow="0" windowWidth="22302" windowHeight="13152" xr2:uid="{9F5D022A-7E51-4F15-A6CA-6252BAE5BCD0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="36">
   <si>
     <t>Dataset</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>To-Do</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -162,7 +165,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,6 +175,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -188,15 +197,77 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -509,7 +580,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -610,8 +681,8 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>34</v>
+      <c r="B6" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>34</v>
@@ -651,7 +722,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>34</v>
@@ -691,7 +762,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>34</v>
@@ -771,7 +842,7 @@
         <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>34</v>
@@ -811,7 +882,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>34</v>
@@ -851,7 +922,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>34</v>
@@ -931,7 +1002,7 @@
         <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>34</v>
@@ -971,7 +1042,7 @@
         <v>25</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>34</v>
@@ -1011,7 +1082,7 @@
         <v>27</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>34</v>
@@ -1087,6 +1158,19 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="To-Do">
+      <formula>NOT(ISERROR(SEARCH("To-Do",B7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:F29">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="To-Do">
+      <formula>NOT(ISERROR(SEARCH("To-Do",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished scala code for AutoMPG Dataset
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CS4360\project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA9DE4F-C914-46E1-A806-5B65CBBAF5DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F8C414-5CA0-42AC-8DD2-6D19F8147AF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22944" yWindow="0" windowWidth="22302" windowHeight="13152" xr2:uid="{9F5D022A-7E51-4F15-A6CA-6252BAE5BCD0}"/>
+    <workbookView xWindow="864" yWindow="-96" windowWidth="22272" windowHeight="13152" xr2:uid="{9F5D022A-7E51-4F15-A6CA-6252BAE5BCD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -206,17 +206,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -224,26 +214,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -580,24 +550,24 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="27.6328125" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.62890625" customWidth="1"/>
+    <col min="2" max="2" width="10.62890625" customWidth="1"/>
+    <col min="3" max="3" width="12.7890625" customWidth="1"/>
+    <col min="5" max="5" width="10.1015625" customWidth="1"/>
+    <col min="6" max="6" width="12.734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -617,7 +587,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -637,7 +607,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -657,7 +627,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -677,7 +647,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -697,12 +667,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>34</v>
@@ -717,7 +687,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -737,12 +707,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>34</v>
@@ -757,7 +727,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -777,12 +747,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>34</v>
@@ -797,7 +767,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -817,7 +787,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -837,7 +807,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -857,12 +827,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>34</v>
@@ -877,7 +847,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -897,12 +867,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>34</v>
@@ -917,7 +887,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -937,12 +907,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>34</v>
@@ -957,7 +927,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -977,7 +947,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -997,7 +967,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1017,12 +987,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>34</v>
@@ -1037,7 +1007,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1057,12 +1027,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>34</v>
@@ -1077,7 +1047,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1097,12 +1067,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>28</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>34</v>
@@ -1117,7 +1087,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1137,7 +1107,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1159,15 +1129,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B7">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="To-Do">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="To-Do">
       <formula>NOT(ISERROR(SEARCH("To-Do",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:F29">
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="To-Do">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="To-Do">
       <formula>NOT(ISERROR(SEARCH("To-Do",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>